<commit_message>
adding excel sheets, changing directories
</commit_message>
<xml_diff>
--- a/Variables_cohorts.xlsx
+++ b/Variables_cohorts.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/med-tv_/Documents/GitHub/KU-COVID-19/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vrw657\Documents\GitHub\KU-COVID-19\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{504378B0-89B9-6640-B450-6893208C7160}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="60" yWindow="460" windowWidth="24240" windowHeight="14020" xr2:uid="{42F559AF-AEA0-714C-9DA4-0B433A5E69ED}"/>
+    <workbookView xWindow="60" yWindow="460" windowWidth="24240" windowHeight="14020"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="107">
   <si>
     <t>Stratifiers</t>
   </si>
@@ -115,9 +114,6 @@
 9. Other</t>
   </si>
   <si>
-    <t>Wat is uw hoogst voltooide opleiding?</t>
-  </si>
-  <si>
     <t>Wat is uw geslacht?</t>
   </si>
   <si>
@@ -168,9 +164,6 @@
   </si>
   <si>
     <t>date</t>
-  </si>
-  <si>
-    <t>Quel est votre diplôme le plus élevé ?</t>
   </si>
   <si>
     <t>1. None
@@ -226,14 +219,6 @@
     <t>1. Male
 2. Female
 3. Other</t>
-  </si>
-  <si>
-    <t>Avez-vous une maladie chronique, c’est-à-dire une maladie qui dure depuis au moins 6 mois et qui peut nécessiter des soins ou un traitement régulier ou un problème de santé ou handicap qui vous limite dans vos activités ?</t>
-  </si>
-  <si>
-    <t>1. Yes
-2. No
-3. I don't know</t>
   </si>
   <si>
     <t>?</t>
@@ -346,64 +331,6 @@
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve">
-Hebt u een chronische aandoening? - </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>If any are selected, YES</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-Hebt u nog een andere aadoening? - </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>If Yes is selected, YES.
-If none of the first options are selected and the answer to the second question is No, then NO.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>2 questions need to be combined:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
 H048 - Tager du regelmæssigt medicin for nogle af følgende sygdomme? Vælg gerne flere svar - </t>
     </r>
     <r>
@@ -470,9 +397,6 @@
   </si>
   <si>
     <t>Likert 1-10</t>
-  </si>
-  <si>
-    <t>How worried are you?</t>
   </si>
   <si>
     <t>Specific worries</t>
@@ -552,29 +476,6 @@
 5. Covering my mouth and nose in public 
 6. Avoiding public transport 
 7. Reduced travel  </t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Ik maak me zorgen om zelf ziek te worden.
-Ik maak me zorgen dat iemand die dichtbij mij staat ziek wordt.
-Ik maak me zorgen dat ik of mijn familie financieel ernstig in de problemen kom(t).
-Ik maak me zorgen dat ik mijn baan verlies.
-Ik maak me zorgen dat het lang gaat duren voordat ik mijn normale. dagelijkse leven weer kan oppakken
-Ik maak me zorgen dat ik familie en vrienden niet kan zien.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>If Sometimes or more, code YES.
-Otherwise code NO for each.</t>
-    </r>
   </si>
   <si>
     <t>Vous sentez-vous inquiet.e au sujet de l’épidémie de coronavirus Covid-19 ?</t>
@@ -624,11 +525,486 @@
   <si>
     <t>NA</t>
   </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Quel est votre diplôme le plus élevé ? </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Please transform this into ~3 categories (corresponding to short/medium/long term education).</t>
+    </r>
+  </si>
+  <si>
+    <t>Mental health</t>
+  </si>
+  <si>
+    <t>Loneliness</t>
+  </si>
+  <si>
+    <t>q16_1, q16_2, q16_3</t>
+  </si>
+  <si>
+    <t>En ce moment, à quelle fréquence vous sentez-vous : 
+(Pour chaque item proposé, les catégories de réponse proposées sont : Jamais ou presque jamais, Parfois, Souvent)</t>
+  </si>
+  <si>
+    <t>Likert 3-9: is combined from 3 questions.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Wat is uw hoogst voltooide opleiding? </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Please transform this into ~3 categories (corresponding to short/medium/long term education).</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>2 questions need to be combined:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Hebt u een chronische aandoening? - </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>If any are selected (except for 12!), YES</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Hebt u nog een andere aadoening? - </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>If Yes is selected, YES.
+If none of the first options are selected and the answer to the second question is No, then NO.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Hebt u een chronische aandoening? - </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>If answer to 12 is Yes, than YES</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Cardiovascular disease (including high blood pressure)
+2. High blood pressure
+3. Heart attack
+4. Narrowing of the arteries in the legs
+5. Stroke or TIA
+6. Other heart and/or coronary diseas
+7. Lung disease, such as asthma, COPD or chronic bronchitis
+8. Liver disease
+9. Kidney disease or reduced kidney function
+10. Diabetes
+11. Chronic muscle disease
+12. Psychological illness, such as depression, psychosis or anxiety disorder
+13. Auto immune illness, usch as celiac disease, inflammatory bowel disorder, rheumatoid arthritis, lupus
+14. Cancer
+15. Neurological disease, such as dementia, Parkinson's disease or Alzheimer disease
+16. Problems with your spleen (e.g. sickle cell anemia, spleen removed)
+</t>
+  </si>
+  <si>
+    <t>q14</t>
+  </si>
+  <si>
+    <t>Kunt u aangeven hoe u zich voelde de afgelopen  7/14 dagen?
+Hoe vaak voelt u zich buitengesloten?
+Hoe vaak voelt u zich afgesloten van anderen?
+Hoe vaak voelt u zich alleen?</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">NA 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>However this is coded, please transform this into ~3 categories (corresponding to short/medium/long term education).</t>
+    </r>
+  </si>
+  <si>
+    <t>Handicap mental ou autres troubles psychiatriques.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2. De quelle(s) maladie(s) ou problème de santé s’agit-il ? (plusieurs réponses possibles)
+If this option is selected, than YES
+</t>
+  </si>
+  <si>
+    <t>1. Yes
+2. No
+3. I don't know
+----------
+Asthme
+Autres maladies respiratoires (bronchite chronique,….)
+Hypertension
+Maladie cardiaque (angine de poitrine, infarctus)
+Diabète
+Troubles digestifs
+Troubles gynécologiques
+Problèmes articulaires, rhumatismes
+Cancer
+Anxiété
+Dépression
+VIH et autres troubles de l’immunité
+Maladies chroniques du foie
+Maladies rénales chroniques
+Handicaps physiques ou aux problèmes physiques
+Handicap mental ou autres troubles psychiatriques
+Autres</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>2 question combined?</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Avez-vous une maladie chronique, c’est-à-dire une maladie qui dure depuis au moins 6 mois et qui peut nécessiter des soins ou un traitement régulier ou un problème de santé ou handicap qui vous limite dans vos activités ?</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+If Yes is selected, than YES
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+2. De quelle(s) maladie(s) ou problème de santé s’agit-il ? (plusieurs réponses possibles)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>If any is selected except for mental disease (Handicap mental ou autres troubles psychiatriques), select YES. Otherwise NO.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+  </si>
+  <si>
+    <t>1.How often do you feel that you lack companionship?
+2. How often do you feel left out?
+3. How often do you feel isolated from others?</t>
+  </si>
+  <si>
+    <t>How often do you feel lonely?</t>
+  </si>
+  <si>
+    <t>1, Hardly ever
+2, Some of the time
+3, Often</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Over the past week, have any of the following been worrying you at all, even if only in a minor way? 
+1, Marriage or other romantic relationship  
+2, Friends or family living in your household  
+3, Friends or family living outside your household  
+4, Neighbours  
+5, Your pet  
+6, Work (even if you feel your job is safe)  
+7, Losing your job / unemployment  
+8, Finances  
+9, Getting medication  
+10, Getting food  
+11, Your own safety / security  
+12, Internet access  
+13, Boredom  
+14, Future plans  
+15, Catching Covid-19  
+16, Becoming seriously ill from Covid-19  
+17, None of these
+</t>
+  </si>
+  <si>
+    <t>Not at all  
+Rarely less than a day or two  
+Several days  
+More than 7 days  
+Nearly every day over the last 2 weeks</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Coronavirus Anxiety Scale - over the past two weeks how anxious have you felt about Covid-19? 
+1. I felt dizzy, lightheaded, or faint, when I read or listened to news about the coronavirus
+2. I had trouble falling or staying asleep because I was thinking about the coronavirus
+3. I felt paralyzed or frozen when I thought about or was exposed to information about the coronavirus
+4. I lost interest in eating when I thought about or was exposed to information about the coronavirus
+5. I felt nauseous or had stomach problems when I thought about or was exposed to information about the coronavirus
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>recode as Yes if More than 7 days or Nearly every day, for each</t>
+    </r>
+  </si>
+  <si>
+    <t>What is your gender?</t>
+  </si>
+  <si>
+    <t>1. Male
+2. Female
+3. Other/Prefer not to say</t>
+  </si>
+  <si>
+    <r>
+      <t>What is your year of birth?</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Please transform this to age filled in at baseline. </t>
+    </r>
+  </si>
+  <si>
+    <t>1, No qualifications
+2, Completed GCSE/CSE/O-levels or equivalent (at school till aged 16)
+3, Completed post-16 vocational course
+4, A-levels or equivalent (at school till aged 18)
+5, Undergraduate degree or professional qualification
+6, Postgraduate degree</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">What is your highest level of educational attainment? </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Please transform this into ~3 categories (corresponding to short/medium/long term education).</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">1, High blood pressure  
+2, Diabetes  
+3, Heart disease  
+4, Lung disease (e.g. asthma or COPD)  
+5, Cancer  
+6, Another clinically-diagnosed chronic physical health condition  
+7, Clinically-diagnosed depression  
+8, Clinically-diagnosed anxiety  
+9, Another clinically-diagnosed mental health problem  
+12, A disability that affects my ability to leave the house  
+13, Any other disability  
+10, I am pregnant  
+11, None of the above
+</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Do you have any of the following medical conditions?
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>If options 7, 8 or 9 are selected, select YES. Otherwise NO.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Do you have any of the following medical conditions?
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>If any are selected except for mental disease (option 7, 8 or 9), select YES. Otherwise NO.</t>
+    </r>
+  </si>
+  <si>
+    <t>UCL Covid-19 Social Study 
+code</t>
+  </si>
+  <si>
+    <t>UCL Covid-19 Social Study
+options</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Ik maak me zorgen om zelf ziek te worden.
+Ik maak me zorgen dat iemand die dichtbij mij staat ziek wordt.
+Ik maak me zorgen dat ik of mijn familie financieel ernstig in de problemen kom(t).
+Ik maak me zorgen dat ik mijn baan verlies.
+Ik maak me zorgen dat het lang gaat duren voordat ik mijn normale. dagelijkse leven weer kan oppakken
+Ik maak me zorgen dat ik familie en vrienden niet kan zien.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>If Frequently or more, code YES.
+Otherwise code NO for each.</t>
+    </r>
+  </si>
+  <si>
+    <t>How worried are you about the corona crisis?</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="5">
     <font>
       <sz val="12"/>
@@ -667,7 +1043,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="12">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -734,6 +1110,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -762,7 +1150,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -873,6 +1261,24 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1188,14 +1594,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0918B519-35F7-354A-8165-CEF3BADB0C0E}">
-  <dimension ref="A1:L10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:N12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G7" workbookViewId="0">
-      <selection activeCell="M9" sqref="M9"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="10.83203125" defaultRowHeight="15.5"/>
   <cols>
     <col min="1" max="1" width="15" style="1" customWidth="1"/>
     <col min="2" max="2" width="13.5" style="1" bestFit="1" customWidth="1"/>
@@ -1209,10 +1615,12 @@
     <col min="10" max="10" width="31.6640625" style="35" customWidth="1"/>
     <col min="11" max="11" width="29.83203125" style="13" customWidth="1"/>
     <col min="12" max="12" width="31.6640625" style="36" customWidth="1"/>
-    <col min="13" max="16384" width="10.83203125" style="1"/>
+    <col min="13" max="13" width="31" style="40" customWidth="1"/>
+    <col min="14" max="14" width="31.9140625" style="43" customWidth="1"/>
+    <col min="15" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="40">
+    <row r="1" spans="1:14" ht="37">
       <c r="A1" s="21" t="s">
         <v>5</v>
       </c>
@@ -1224,10 +1632,10 @@
         <v>8</v>
       </c>
       <c r="E1" s="24" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="F1" s="25" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="G1" s="26" t="s">
         <v>18</v>
@@ -1236,19 +1644,25 @@
         <v>16</v>
       </c>
       <c r="I1" s="28" t="s">
+        <v>23</v>
+      </c>
+      <c r="J1" s="29" t="s">
         <v>24</v>
       </c>
-      <c r="J1" s="29" t="s">
-        <v>25</v>
-      </c>
       <c r="K1" s="30" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="L1" s="31" t="s">
-        <v>35</v>
+        <v>33</v>
+      </c>
+      <c r="M1" s="38" t="s">
+        <v>104</v>
+      </c>
+      <c r="N1" s="41" t="s">
+        <v>103</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="68">
+    <row r="2" spans="1:14" ht="46.5">
       <c r="A2" s="21" t="s">
         <v>0</v>
       </c>
@@ -1265,28 +1679,34 @@
         <v>19</v>
       </c>
       <c r="F2" s="18" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H2" s="10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I2" s="11" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="J2" s="12" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="K2" s="15" t="s">
         <v>19</v>
       </c>
       <c r="L2" s="16" t="s">
-        <v>36</v>
+        <v>34</v>
+      </c>
+      <c r="M2" s="39" t="s">
+        <v>28</v>
+      </c>
+      <c r="N2" s="42" t="s">
+        <v>97</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="68">
+    <row r="3" spans="1:14" ht="62">
       <c r="A3" s="8"/>
       <c r="B3" s="8" t="s">
         <v>2</v>
@@ -1301,28 +1721,34 @@
         <v>12</v>
       </c>
       <c r="F3" s="18" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="G3" s="6" t="s">
         <v>15</v>
       </c>
       <c r="H3" s="10" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I3" s="11" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="J3" s="12" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="K3" s="15" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="L3" s="16" t="s">
-        <v>37</v>
+        <v>35</v>
+      </c>
+      <c r="M3" s="39" t="s">
+        <v>96</v>
+      </c>
+      <c r="N3" s="42" t="s">
+        <v>95</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="221">
+    <row r="4" spans="1:14" ht="201.5">
       <c r="A4" s="8"/>
       <c r="B4" s="8" t="s">
         <v>3</v>
@@ -1337,28 +1763,34 @@
         <v>11</v>
       </c>
       <c r="F4" s="19" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="G4" s="6" t="s">
         <v>20</v>
       </c>
       <c r="H4" s="10" t="s">
-        <v>21</v>
+        <v>78</v>
       </c>
       <c r="I4" s="11" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="J4" s="12" t="s">
-        <v>30</v>
+        <v>72</v>
       </c>
       <c r="K4" s="15" t="s">
-        <v>41</v>
+        <v>71</v>
       </c>
       <c r="L4" s="16" t="s">
-        <v>41</v>
+        <v>84</v>
+      </c>
+      <c r="M4" s="39" t="s">
+        <v>98</v>
+      </c>
+      <c r="N4" s="42" t="s">
+        <v>99</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="409" customHeight="1">
+    <row r="5" spans="1:14" ht="409.5">
       <c r="A5" s="8"/>
       <c r="B5" s="8" t="s">
         <v>4</v>
@@ -1370,180 +1802,289 @@
         <v>7</v>
       </c>
       <c r="E5" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="F5" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="G5" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="H5" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="I5" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="J5" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="K5" s="15" t="s">
+        <v>87</v>
+      </c>
+      <c r="L5" s="16" t="s">
+        <v>88</v>
+      </c>
+      <c r="M5" s="39" t="s">
+        <v>100</v>
+      </c>
+      <c r="N5" s="42" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" ht="341">
+      <c r="A6" s="8"/>
+      <c r="B6" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="C6" s="37" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="E6" s="17"/>
+      <c r="F6" s="18"/>
+      <c r="G6" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="H6" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="I6" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="J6" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="K6" s="15" t="s">
+        <v>85</v>
+      </c>
+      <c r="L6" s="16" t="s">
+        <v>86</v>
+      </c>
+      <c r="M6" s="39" t="s">
+        <v>100</v>
+      </c>
+      <c r="N6" s="42" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" ht="62">
+      <c r="A7" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="C7" s="20" t="s">
         <v>48</v>
       </c>
-      <c r="F5" s="18" t="s">
-        <v>50</v>
-      </c>
-      <c r="G5" s="6" t="s">
+      <c r="D7" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="H5" s="10" t="s">
-        <v>49</v>
-      </c>
-      <c r="I5" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="J5" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="K5" s="15" t="s">
-        <v>40</v>
-      </c>
-      <c r="L5" s="16" t="s">
-        <v>39</v>
+      <c r="E7" s="17" t="s">
+        <v>48</v>
+      </c>
+      <c r="F7" s="18" t="s">
+        <v>56</v>
+      </c>
+      <c r="G7" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="H7" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="I7" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="J7" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="K7" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="L7" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="M7" s="39" t="s">
+        <v>91</v>
+      </c>
+      <c r="N7" s="42" t="s">
+        <v>90</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="68">
-      <c r="A6" s="21" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="C6" s="20" t="s">
-        <v>53</v>
-      </c>
-      <c r="D6" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="E6" s="17" t="s">
-        <v>53</v>
-      </c>
-      <c r="F6" s="18" t="s">
-        <v>62</v>
-      </c>
-      <c r="G6" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="H6" s="10" t="s">
-        <v>65</v>
-      </c>
-      <c r="I6" s="11" t="s">
-        <v>53</v>
-      </c>
-      <c r="J6" s="12" t="s">
+    <row r="8" spans="1:14" ht="132" customHeight="1">
+      <c r="A8" s="21"/>
+      <c r="B8" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="C8" s="20" t="s">
+        <v>77</v>
+      </c>
+      <c r="D8" s="9" t="s">
         <v>75</v>
       </c>
-      <c r="K6" s="15" t="s">
-        <v>78</v>
-      </c>
-      <c r="L6" s="16" t="s">
-        <v>78</v>
+      <c r="E8" s="17" t="s">
+        <v>77</v>
+      </c>
+      <c r="F8" s="18"/>
+      <c r="G8" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="H8" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="I8" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="J8" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="K8" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="L8" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="M8" s="39" t="s">
+        <v>77</v>
+      </c>
+      <c r="N8" s="42" t="s">
+        <v>89</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="136">
-      <c r="A7" s="8"/>
-      <c r="B7" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="C7" s="20" t="s">
-        <v>53</v>
-      </c>
-      <c r="D7" s="9" t="s">
-        <v>57</v>
-      </c>
-      <c r="E7" s="17" t="s">
-        <v>53</v>
-      </c>
-      <c r="F7" s="18" t="s">
-        <v>61</v>
-      </c>
-      <c r="G7" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="H7" s="10" t="s">
-        <v>66</v>
-      </c>
-      <c r="I7" s="11" t="s">
-        <v>72</v>
-      </c>
-      <c r="J7" s="12" t="s">
-        <v>71</v>
-      </c>
-      <c r="K7" s="15" t="s">
-        <v>77</v>
-      </c>
-      <c r="L7" s="16" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" ht="340">
-      <c r="A8" s="8"/>
-      <c r="B8" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="D8" s="9" t="s">
-        <v>58</v>
-      </c>
-      <c r="E8" s="17" t="s">
-        <v>60</v>
-      </c>
-      <c r="F8" s="18" t="s">
-        <v>63</v>
-      </c>
-      <c r="G8" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="H8" s="10" t="s">
-        <v>70</v>
-      </c>
-      <c r="I8" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="J8" s="12" t="s">
-        <v>73</v>
-      </c>
-      <c r="K8" s="15" t="s">
-        <v>41</v>
-      </c>
-      <c r="L8" s="16" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" ht="255">
+    <row r="9" spans="1:14" ht="341">
       <c r="A9" s="8"/>
       <c r="B9" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="C9" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="C9" s="20" t="s">
+        <v>48</v>
+      </c>
+      <c r="D9" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="E9" s="17" t="s">
+        <v>48</v>
+      </c>
+      <c r="F9" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="G9" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="H9" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="D9" s="9" t="s">
-        <v>59</v>
-      </c>
-      <c r="E9" s="17" t="s">
-        <v>60</v>
-      </c>
-      <c r="F9" s="18" t="s">
+      <c r="I9" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="J9" s="12" t="s">
         <v>64</v>
       </c>
-      <c r="G9" s="6" t="s">
+      <c r="K9" s="15" t="s">
+        <v>70</v>
+      </c>
+      <c r="L9" s="16" t="s">
         <v>69</v>
       </c>
-      <c r="H9" s="10" t="s">
-        <v>68</v>
-      </c>
-      <c r="I9" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="J9" s="12" t="s">
-        <v>74</v>
-      </c>
-      <c r="K9" s="15" t="s">
-        <v>41</v>
-      </c>
-      <c r="L9" s="16" t="s">
-        <v>41</v>
+      <c r="M9" s="39" t="s">
+        <v>93</v>
+      </c>
+      <c r="N9" s="42" t="s">
+        <v>94</v>
       </c>
     </row>
-    <row r="10" spans="1:12">
-      <c r="L10" s="14"/>
+    <row r="10" spans="1:14" ht="403">
+      <c r="A10" s="8"/>
+      <c r="B10" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="D10" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="E10" s="17" t="s">
+        <v>54</v>
+      </c>
+      <c r="F10" s="18" t="s">
+        <v>57</v>
+      </c>
+      <c r="G10" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="H10" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="I10" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="J10" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="K10" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="L10" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="M10" s="39" t="s">
+        <v>54</v>
+      </c>
+      <c r="N10" s="42" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" ht="232.5">
+      <c r="A11" s="8"/>
+      <c r="B11" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="D11" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="E11" s="17" t="s">
+        <v>54</v>
+      </c>
+      <c r="F11" s="18" t="s">
+        <v>58</v>
+      </c>
+      <c r="G11" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="H11" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="I11" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="J11" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="K11" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="L11" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="M11" s="39" t="s">
+        <v>71</v>
+      </c>
+      <c r="N11" s="42" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14">
+      <c r="L12" s="14"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
DNBC script - adding mental health and chronic disease
</commit_message>
<xml_diff>
--- a/Variables_cohorts.xlsx
+++ b/Variables_cohorts.xlsx
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="109">
   <si>
     <t>Stratifiers</t>
   </si>
@@ -999,6 +999,12 @@
   </si>
   <si>
     <t>How worried are you about the corona crisis?</t>
+  </si>
+  <si>
+    <t>H052</t>
+  </si>
+  <si>
+    <t>"H057", "H058", "H059"</t>
   </si>
 </sst>
 </file>
@@ -1597,8 +1603,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H9" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="L9" sqref="L9"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.83203125" defaultRowHeight="15.5"/>
@@ -1844,7 +1850,9 @@
         <v>82</v>
       </c>
       <c r="E6" s="17"/>
-      <c r="F6" s="18"/>
+      <c r="F6" s="18" t="s">
+        <v>107</v>
+      </c>
       <c r="G6" s="6" t="s">
         <v>81</v>
       </c>
@@ -1928,7 +1936,9 @@
       <c r="E8" s="17" t="s">
         <v>77</v>
       </c>
-      <c r="F8" s="18"/>
+      <c r="F8" s="18" t="s">
+        <v>108</v>
+      </c>
       <c r="G8" s="6" t="s">
         <v>77</v>
       </c>

</xml_diff>